<commit_message>
Updated timesheet and Register page component
</commit_message>
<xml_diff>
--- a/Process/Timesheet/Timesheet 2.xlsx
+++ b/Process/Timesheet/Timesheet 2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aspire\GIT-Rafi_Project\Project\Process\Timesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vinoth\GIT\TeamProject\Project\Process\Timesheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA52455B-7CFC-4C74-96EA-62810423D57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="30" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23263" windowHeight="12463" firstSheet="30" activeTab="32"/>
   </bookViews>
   <sheets>
     <sheet name="Day 3(06-04-2022)" sheetId="40" r:id="rId1"/>
@@ -47,7 +46,7 @@
     <sheet name="Day31(16-05-2022)-Monday's" sheetId="78" r:id="rId32"/>
     <sheet name="Day32(17-05-2022)-Tuesday's" sheetId="79" r:id="rId33"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5754" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5752" uniqueCount="1081">
   <si>
     <t>Column1</t>
   </si>
@@ -3751,11 +3750,17 @@
   <si>
     <t>Attended Planning Meet with Rafi</t>
   </si>
+  <si>
+    <t xml:space="preserve">Worked on register page </t>
+  </si>
+  <si>
+    <t>Angular session with saraswathi (HTTP POST)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]hh:mm:ss;@"/>
   </numFmts>
@@ -15524,464 +15529,464 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="621" dataDxfId="619" headerRowBorderDxfId="620" tableBorderDxfId="618" totalsRowBorderDxfId="617">
-  <autoFilter ref="B9:H19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B9:H19" totalsRowShown="0" headerRowDxfId="621" dataDxfId="619" headerRowBorderDxfId="620" tableBorderDxfId="618" totalsRowBorderDxfId="617">
+  <autoFilter ref="B9:H19"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Resource Name" dataDxfId="616"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-progress" dataDxfId="615"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Done" dataDxfId="614"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Discarded / Hold" dataDxfId="613"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Hours Spent - Project" dataDxfId="612"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Hours Spent - Non Project" dataDxfId="611"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="610"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="616"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="615"/>
+    <tableColumn id="3" name="Done" dataDxfId="614"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="613"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="612"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="611"/>
+    <tableColumn id="7" name="Comments" dataDxfId="610"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="525" dataDxfId="523" headerRowBorderDxfId="524" tableBorderDxfId="522" totalsRowBorderDxfId="521">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table3751113" displayName="Table3751113" ref="B2:E4" totalsRowShown="0" headerRowDxfId="525" dataDxfId="523" headerRowBorderDxfId="524" tableBorderDxfId="522" totalsRowBorderDxfId="521">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Column1" dataDxfId="520"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Column2" dataDxfId="519"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Column3" dataDxfId="518"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Column4" dataDxfId="517"/>
+    <tableColumn id="1" name="Column1" dataDxfId="520"/>
+    <tableColumn id="2" name="Column2" dataDxfId="519"/>
+    <tableColumn id="3" name="Column3" dataDxfId="518"/>
+    <tableColumn id="4" name="Column4" dataDxfId="517"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="516" dataDxfId="514" headerRowBorderDxfId="515" tableBorderDxfId="513" totalsRowBorderDxfId="512">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table2621014" displayName="Table2621014" ref="B7:H17" totalsRowShown="0" headerRowDxfId="516" dataDxfId="514" headerRowBorderDxfId="515" tableBorderDxfId="513" totalsRowBorderDxfId="512">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Resource Name" dataDxfId="511"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="In-progress" dataDxfId="510"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Done" dataDxfId="509"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Discarded / Hold" dataDxfId="508"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Hours Spent - Project" dataDxfId="507"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Hours Spent - Non Project" dataDxfId="506"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="Comments" dataDxfId="505"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="511"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="510"/>
+    <tableColumn id="3" name="Done" dataDxfId="509"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="508"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="507"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="506"/>
+    <tableColumn id="7" name="Comments" dataDxfId="505"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="504" dataDxfId="502" headerRowBorderDxfId="503" tableBorderDxfId="501" totalsRowBorderDxfId="500">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table3751115" displayName="Table3751115" ref="B2:E4" totalsRowShown="0" headerRowDxfId="504" dataDxfId="502" headerRowBorderDxfId="503" tableBorderDxfId="501" totalsRowBorderDxfId="500">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Column1" dataDxfId="499"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Column2" dataDxfId="498"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Column3" dataDxfId="497"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Column4" dataDxfId="496"/>
+    <tableColumn id="1" name="Column1" dataDxfId="499"/>
+    <tableColumn id="2" name="Column2" dataDxfId="498"/>
+    <tableColumn id="3" name="Column3" dataDxfId="497"/>
+    <tableColumn id="4" name="Column4" dataDxfId="496"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="495" dataDxfId="493" headerRowBorderDxfId="494" tableBorderDxfId="492" totalsRowBorderDxfId="491">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table26210" displayName="Table26210" ref="B7:H17" totalsRowShown="0" headerRowDxfId="495" dataDxfId="493" headerRowBorderDxfId="494" tableBorderDxfId="492" totalsRowBorderDxfId="491">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Resource Name" dataDxfId="490"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="In-progress" dataDxfId="489"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Done" dataDxfId="488"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Discarded / Hold" dataDxfId="487"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Hours Spent - Project" dataDxfId="486"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Hours Spent - Non Project" dataDxfId="485"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Comments" dataDxfId="484"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="490"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="489"/>
+    <tableColumn id="3" name="Done" dataDxfId="488"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="487"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="486"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="485"/>
+    <tableColumn id="7" name="Comments" dataDxfId="484"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="483" dataDxfId="481" headerRowBorderDxfId="482" tableBorderDxfId="480" totalsRowBorderDxfId="479">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table37511" displayName="Table37511" ref="B2:E4" totalsRowShown="0" headerRowDxfId="483" dataDxfId="481" headerRowBorderDxfId="482" tableBorderDxfId="480" totalsRowBorderDxfId="479">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Column1" dataDxfId="478"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Column2" dataDxfId="477"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Column3" dataDxfId="476"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Column4" dataDxfId="475"/>
+    <tableColumn id="1" name="Column1" dataDxfId="478"/>
+    <tableColumn id="2" name="Column2" dataDxfId="477"/>
+    <tableColumn id="3" name="Column3" dataDxfId="476"/>
+    <tableColumn id="4" name="Column4" dataDxfId="475"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="474" dataDxfId="472" headerRowBorderDxfId="473" tableBorderDxfId="471" totalsRowBorderDxfId="470">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table2621016" displayName="Table2621016" ref="B7:H17" totalsRowShown="0" headerRowDxfId="474" dataDxfId="472" headerRowBorderDxfId="473" tableBorderDxfId="471" totalsRowBorderDxfId="470">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Resource Name" dataDxfId="469"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="In-progress" dataDxfId="468"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="Done" dataDxfId="467"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Discarded / Hold" dataDxfId="466"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Hours Spent - Project" dataDxfId="465"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Hours Spent - Non Project" dataDxfId="464"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="Comments" dataDxfId="463"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="469"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="468"/>
+    <tableColumn id="3" name="Done" dataDxfId="467"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="466"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="465"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="464"/>
+    <tableColumn id="7" name="Comments" dataDxfId="463"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="462" dataDxfId="460" headerRowBorderDxfId="461" tableBorderDxfId="459" totalsRowBorderDxfId="458">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table3751117" displayName="Table3751117" ref="B2:E4" totalsRowShown="0" headerRowDxfId="462" dataDxfId="460" headerRowBorderDxfId="461" tableBorderDxfId="459" totalsRowBorderDxfId="458">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Column1" dataDxfId="457"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="Column2" dataDxfId="456"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="Column3" dataDxfId="455"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="Column4" dataDxfId="454"/>
+    <tableColumn id="1" name="Column1" dataDxfId="457"/>
+    <tableColumn id="2" name="Column2" dataDxfId="456"/>
+    <tableColumn id="3" name="Column3" dataDxfId="455"/>
+    <tableColumn id="4" name="Column4" dataDxfId="454"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="453" dataDxfId="451" headerRowBorderDxfId="452" tableBorderDxfId="450" totalsRowBorderDxfId="449">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table262101618" displayName="Table262101618" ref="B7:H17" totalsRowShown="0" headerRowDxfId="453" dataDxfId="451" headerRowBorderDxfId="452" tableBorderDxfId="450" totalsRowBorderDxfId="449">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Resource Name" dataDxfId="448"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="In-progress" dataDxfId="447"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="Done" dataDxfId="446"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="Discarded / Hold" dataDxfId="445"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Hours Spent - Project" dataDxfId="444"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="Hours Spent - Non Project" dataDxfId="443"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="Comments" dataDxfId="442"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="448"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="447"/>
+    <tableColumn id="3" name="Done" dataDxfId="446"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="445"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="444"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="443"/>
+    <tableColumn id="7" name="Comments" dataDxfId="442"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="441" dataDxfId="439" headerRowBorderDxfId="440" tableBorderDxfId="438" totalsRowBorderDxfId="437">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table375111719" displayName="Table375111719" ref="B2:E4" totalsRowShown="0" headerRowDxfId="441" dataDxfId="439" headerRowBorderDxfId="440" tableBorderDxfId="438" totalsRowBorderDxfId="437">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Column1" dataDxfId="436"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="Column2" dataDxfId="435"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="Column3" dataDxfId="434"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="Column4" dataDxfId="433"/>
+    <tableColumn id="1" name="Column1" dataDxfId="436"/>
+    <tableColumn id="2" name="Column2" dataDxfId="435"/>
+    <tableColumn id="3" name="Column3" dataDxfId="434"/>
+    <tableColumn id="4" name="Column4" dataDxfId="433"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="432" dataDxfId="430" headerRowBorderDxfId="431" tableBorderDxfId="429" totalsRowBorderDxfId="428">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table26210161820" displayName="Table26210161820" ref="B7:H17" totalsRowShown="0" headerRowDxfId="432" dataDxfId="430" headerRowBorderDxfId="431" tableBorderDxfId="429" totalsRowBorderDxfId="428">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Resource Name" dataDxfId="427"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="In-progress" dataDxfId="426"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="Done" dataDxfId="425"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="Discarded / Hold" dataDxfId="424"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="Hours Spent - Project" dataDxfId="423"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="Hours Spent - Non Project" dataDxfId="422"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="Comments" dataDxfId="421"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="427"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="426"/>
+    <tableColumn id="3" name="Done" dataDxfId="425"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="424"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="423"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="422"/>
+    <tableColumn id="7" name="Comments" dataDxfId="421"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="609" dataDxfId="607" headerRowBorderDxfId="608" tableBorderDxfId="606" totalsRowBorderDxfId="605">
-  <autoFilter ref="B4:E6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:E6" totalsRowShown="0" headerRowDxfId="609" dataDxfId="607" headerRowBorderDxfId="608" tableBorderDxfId="606" totalsRowBorderDxfId="605">
+  <autoFilter ref="B4:E6"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="604"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="603"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3" dataDxfId="602"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4" dataDxfId="601"/>
+    <tableColumn id="1" name="Column1" dataDxfId="604"/>
+    <tableColumn id="2" name="Column2" dataDxfId="603"/>
+    <tableColumn id="3" name="Column3" dataDxfId="602"/>
+    <tableColumn id="4" name="Column4" dataDxfId="601"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="420" dataDxfId="418" headerRowBorderDxfId="419" tableBorderDxfId="417" totalsRowBorderDxfId="416">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table37511171921" displayName="Table37511171921" ref="B2:E4" totalsRowShown="0" headerRowDxfId="420" dataDxfId="418" headerRowBorderDxfId="419" tableBorderDxfId="417" totalsRowBorderDxfId="416">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Column1" dataDxfId="415"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="Column2" dataDxfId="414"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="Column3" dataDxfId="413"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="Column4" dataDxfId="412"/>
+    <tableColumn id="1" name="Column1" dataDxfId="415"/>
+    <tableColumn id="2" name="Column2" dataDxfId="414"/>
+    <tableColumn id="3" name="Column3" dataDxfId="413"/>
+    <tableColumn id="4" name="Column4" dataDxfId="412"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Table2621016182022" displayName="Table2621016182022" ref="B7:H17" totalsRowShown="0" headerRowDxfId="411" dataDxfId="409" headerRowBorderDxfId="410" tableBorderDxfId="408" totalsRowBorderDxfId="407">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2621016182022" displayName="Table2621016182022" ref="B7:H17" totalsRowShown="0" headerRowDxfId="411" dataDxfId="409" headerRowBorderDxfId="410" tableBorderDxfId="408" totalsRowBorderDxfId="407">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Resource Name" dataDxfId="406"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="In-progress" dataDxfId="405"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="Done" dataDxfId="404"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="Discarded / Hold" dataDxfId="403"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="Hours Spent - Project" dataDxfId="402"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="Hours Spent - Non Project" dataDxfId="401"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1400-000007000000}" name="Comments" dataDxfId="400"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="406"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="405"/>
+    <tableColumn id="3" name="Done" dataDxfId="404"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="403"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="402"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="401"/>
+    <tableColumn id="7" name="Comments" dataDxfId="400"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Table3751117192123" displayName="Table3751117192123" ref="B2:E4" totalsRowShown="0" headerRowDxfId="399" dataDxfId="397" headerRowBorderDxfId="398" tableBorderDxfId="396" totalsRowBorderDxfId="395">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table3751117192123" displayName="Table3751117192123" ref="B2:E4" totalsRowShown="0" headerRowDxfId="399" dataDxfId="397" headerRowBorderDxfId="398" tableBorderDxfId="396" totalsRowBorderDxfId="395">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Column1" dataDxfId="394"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="Column2" dataDxfId="393"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="Column3" dataDxfId="392"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="Column4" dataDxfId="391"/>
+    <tableColumn id="1" name="Column1" dataDxfId="394"/>
+    <tableColumn id="2" name="Column2" dataDxfId="393"/>
+    <tableColumn id="3" name="Column3" dataDxfId="392"/>
+    <tableColumn id="4" name="Column4" dataDxfId="391"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Table26210161820222426" displayName="Table26210161820222426" ref="B7:H17" totalsRowShown="0" headerRowDxfId="390" dataDxfId="388" headerRowBorderDxfId="389" tableBorderDxfId="387" totalsRowBorderDxfId="386">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table26210161820222426" displayName="Table26210161820222426" ref="B7:H17" totalsRowShown="0" headerRowDxfId="390" dataDxfId="388" headerRowBorderDxfId="389" tableBorderDxfId="387" totalsRowBorderDxfId="386">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Resource Name" dataDxfId="385"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="In-progress" dataDxfId="384"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="Done" dataDxfId="383"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="Discarded / Hold" dataDxfId="382"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="Hours Spent - Project" dataDxfId="381"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="Hours Spent - Non Project" dataDxfId="380"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="Comments" dataDxfId="379"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="385"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="384"/>
+    <tableColumn id="3" name="Done" dataDxfId="383"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="382"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="381"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="380"/>
+    <tableColumn id="7" name="Comments" dataDxfId="379"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="Table37511171921232527" displayName="Table37511171921232527" ref="B2:E4" totalsRowShown="0" headerRowDxfId="378" dataDxfId="376" headerRowBorderDxfId="377" tableBorderDxfId="375" totalsRowBorderDxfId="374">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table37511171921232527" displayName="Table37511171921232527" ref="B2:E4" totalsRowShown="0" headerRowDxfId="378" dataDxfId="376" headerRowBorderDxfId="377" tableBorderDxfId="375" totalsRowBorderDxfId="374">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Column1" dataDxfId="373"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="Column2" dataDxfId="372"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1700-000003000000}" name="Column3" dataDxfId="371"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1700-000004000000}" name="Column4" dataDxfId="370"/>
+    <tableColumn id="1" name="Column1" dataDxfId="373"/>
+    <tableColumn id="2" name="Column2" dataDxfId="372"/>
+    <tableColumn id="3" name="Column3" dataDxfId="371"/>
+    <tableColumn id="4" name="Column4" dataDxfId="370"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="Table262101618202224" displayName="Table262101618202224" ref="B7:H17" totalsRowShown="0" headerRowDxfId="369" dataDxfId="367" headerRowBorderDxfId="368" tableBorderDxfId="366" totalsRowBorderDxfId="365">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table262101618202224" displayName="Table262101618202224" ref="B7:H17" totalsRowShown="0" headerRowDxfId="369" dataDxfId="367" headerRowBorderDxfId="368" tableBorderDxfId="366" totalsRowBorderDxfId="365">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Resource Name" dataDxfId="364"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="In-progress" dataDxfId="363"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="Done" dataDxfId="362"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="Discarded / Hold" dataDxfId="361"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="Hours Spent - Project" dataDxfId="360"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="Hours Spent - Non Project" dataDxfId="359"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1800-000007000000}" name="Comments" dataDxfId="358"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="364"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="363"/>
+    <tableColumn id="3" name="Done" dataDxfId="362"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="361"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="360"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="359"/>
+    <tableColumn id="7" name="Comments" dataDxfId="358"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="Table375111719212325" displayName="Table375111719212325" ref="B2:E4" totalsRowShown="0" headerRowDxfId="357" dataDxfId="355" headerRowBorderDxfId="356" tableBorderDxfId="354" totalsRowBorderDxfId="353">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Table375111719212325" displayName="Table375111719212325" ref="B2:E4" totalsRowShown="0" headerRowDxfId="357" dataDxfId="355" headerRowBorderDxfId="356" tableBorderDxfId="354" totalsRowBorderDxfId="353">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Column1" dataDxfId="352"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="Column2" dataDxfId="351"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="Column3" dataDxfId="350"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="Column4" dataDxfId="349"/>
+    <tableColumn id="1" name="Column1" dataDxfId="352"/>
+    <tableColumn id="2" name="Column2" dataDxfId="351"/>
+    <tableColumn id="3" name="Column3" dataDxfId="350"/>
+    <tableColumn id="4" name="Column4" dataDxfId="349"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="Table2621016182022242830" displayName="Table2621016182022242830" ref="B9:H19" totalsRowShown="0" headerRowDxfId="348" dataDxfId="346" headerRowBorderDxfId="347" tableBorderDxfId="345" totalsRowBorderDxfId="344">
-  <autoFilter ref="B9:H19" xr:uid="{00000000-0009-0000-0100-00001D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table2621016182022242830" displayName="Table2621016182022242830" ref="B9:H19" totalsRowShown="0" headerRowDxfId="348" dataDxfId="346" headerRowBorderDxfId="347" tableBorderDxfId="345" totalsRowBorderDxfId="344">
+  <autoFilter ref="B9:H19"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="Resource Name" dataDxfId="343"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="In-progress" dataDxfId="342"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1A00-000003000000}" name="Done" dataDxfId="341"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="Discarded / Hold" dataDxfId="340"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1A00-000005000000}" name="Hours Spent - Project" dataDxfId="339"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1A00-000006000000}" name="Hours Spent - Non Project" dataDxfId="338"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1A00-000007000000}" name="Comments" dataDxfId="337"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="343"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="342"/>
+    <tableColumn id="3" name="Done" dataDxfId="341"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="340"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="339"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="338"/>
+    <tableColumn id="7" name="Comments" dataDxfId="337"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="Table3751117192123252931" displayName="Table3751117192123252931" ref="B4:E6" totalsRowShown="0" headerRowDxfId="336" dataDxfId="334" headerRowBorderDxfId="335" tableBorderDxfId="333" totalsRowBorderDxfId="332">
-  <autoFilter ref="B4:E6" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Table3751117192123252931" displayName="Table3751117192123252931" ref="B4:E6" totalsRowShown="0" headerRowDxfId="336" dataDxfId="334" headerRowBorderDxfId="335" tableBorderDxfId="333" totalsRowBorderDxfId="332">
+  <autoFilter ref="B4:E6"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="Column1" dataDxfId="331"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="Column2" dataDxfId="330"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="Column3" dataDxfId="329"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1B00-000004000000}" name="Column4" dataDxfId="328"/>
+    <tableColumn id="1" name="Column1" dataDxfId="331"/>
+    <tableColumn id="2" name="Column2" dataDxfId="330"/>
+    <tableColumn id="3" name="Column3" dataDxfId="329"/>
+    <tableColumn id="4" name="Column4" dataDxfId="328"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="Table26210161820222428" displayName="Table26210161820222428" ref="B9:H19" totalsRowShown="0" headerRowDxfId="327" dataDxfId="325" headerRowBorderDxfId="326" tableBorderDxfId="324" totalsRowBorderDxfId="323">
-  <autoFilter ref="B9:H19" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table26210161820222428" displayName="Table26210161820222428" ref="B9:H19" totalsRowShown="0" headerRowDxfId="327" dataDxfId="325" headerRowBorderDxfId="326" tableBorderDxfId="324" totalsRowBorderDxfId="323">
+  <autoFilter ref="B9:H19"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="Resource Name" dataDxfId="322"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="In-progress" dataDxfId="321"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1C00-000003000000}" name="Done" dataDxfId="320"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1C00-000004000000}" name="Discarded / Hold" dataDxfId="319"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="Hours Spent - Project" dataDxfId="318"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1C00-000006000000}" name="Hours Spent - Non Project" dataDxfId="317"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1C00-000007000000}" name="Comments" dataDxfId="316"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="322"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="321"/>
+    <tableColumn id="3" name="Done" dataDxfId="320"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="319"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="318"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="317"/>
+    <tableColumn id="7" name="Comments" dataDxfId="316"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="600" dataDxfId="598" headerRowBorderDxfId="599" tableBorderDxfId="597" totalsRowBorderDxfId="596">
-  <autoFilter ref="B8:H18" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="B8:H18" totalsRowShown="0" headerRowDxfId="600" dataDxfId="598" headerRowBorderDxfId="599" tableBorderDxfId="597" totalsRowBorderDxfId="596">
+  <autoFilter ref="B8:H18"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Resource Name" dataDxfId="595"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="In-progress" dataDxfId="594"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Done" dataDxfId="593"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Discarded / Hold" dataDxfId="592"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Hours Spent - Project" dataDxfId="591"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Hours Spent - Non Project" dataDxfId="590"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Comments" dataDxfId="589"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="595"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="594"/>
+    <tableColumn id="3" name="Done" dataDxfId="593"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="592"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="591"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="590"/>
+    <tableColumn id="7" name="Comments" dataDxfId="589"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="Table37511171921232529" displayName="Table37511171921232529" ref="B4:E6" totalsRowShown="0" headerRowDxfId="315" dataDxfId="313" headerRowBorderDxfId="314" tableBorderDxfId="312" totalsRowBorderDxfId="311">
-  <autoFilter ref="B4:E6" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table37511171921232529" displayName="Table37511171921232529" ref="B4:E6" totalsRowShown="0" headerRowDxfId="315" dataDxfId="313" headerRowBorderDxfId="314" tableBorderDxfId="312" totalsRowBorderDxfId="311">
+  <autoFilter ref="B4:E6"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="Column1" dataDxfId="310"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="Column2" dataDxfId="309"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="Column3" dataDxfId="308"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1D00-000004000000}" name="Column4" dataDxfId="307"/>
+    <tableColumn id="1" name="Column1" dataDxfId="310"/>
+    <tableColumn id="2" name="Column2" dataDxfId="309"/>
+    <tableColumn id="3" name="Column3" dataDxfId="308"/>
+    <tableColumn id="4" name="Column4" dataDxfId="307"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF1E000000}" name="Table262101618202224283234" displayName="Table262101618202224283234" ref="B9:H19" totalsRowShown="0" headerRowDxfId="306" dataDxfId="304" headerRowBorderDxfId="305" tableBorderDxfId="303" totalsRowBorderDxfId="302">
-  <autoFilter ref="B9:H19" xr:uid="{00000000-0009-0000-0100-000021000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Table262101618202224283234" displayName="Table262101618202224283234" ref="B9:H19" totalsRowShown="0" headerRowDxfId="306" dataDxfId="304" headerRowBorderDxfId="305" tableBorderDxfId="303" totalsRowBorderDxfId="302">
+  <autoFilter ref="B9:H19"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1E00-000001000000}" name="Resource Name" dataDxfId="301"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1E00-000002000000}" name="In-progress" dataDxfId="300"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1E00-000003000000}" name="Done" dataDxfId="299"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1E00-000004000000}" name="Discarded / Hold" dataDxfId="298"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1E00-000005000000}" name="Hours Spent - Project" dataDxfId="297"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1E00-000006000000}" name="Hours Spent - Non Project" dataDxfId="296"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1E00-000007000000}" name="Comments" dataDxfId="295"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="301"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="300"/>
+    <tableColumn id="3" name="Done" dataDxfId="299"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="298"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="297"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="296"/>
+    <tableColumn id="7" name="Comments" dataDxfId="295"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="Table375111719212325293335" displayName="Table375111719212325293335" ref="B4:E6" totalsRowShown="0" headerRowDxfId="294" dataDxfId="292" headerRowBorderDxfId="293" tableBorderDxfId="291" totalsRowBorderDxfId="290">
-  <autoFilter ref="B4:E6" xr:uid="{00000000-0009-0000-0100-000022000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="Table375111719212325293335" displayName="Table375111719212325293335" ref="B4:E6" totalsRowShown="0" headerRowDxfId="294" dataDxfId="292" headerRowBorderDxfId="293" tableBorderDxfId="291" totalsRowBorderDxfId="290">
+  <autoFilter ref="B4:E6"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="Column1" dataDxfId="289"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="Column2" dataDxfId="288"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1F00-000003000000}" name="Column3" dataDxfId="287"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1F00-000004000000}" name="Column4" dataDxfId="286"/>
+    <tableColumn id="1" name="Column1" dataDxfId="289"/>
+    <tableColumn id="2" name="Column2" dataDxfId="288"/>
+    <tableColumn id="3" name="Column3" dataDxfId="287"/>
+    <tableColumn id="4" name="Column4" dataDxfId="286"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="588" dataDxfId="586" headerRowBorderDxfId="587" tableBorderDxfId="585" totalsRowBorderDxfId="584">
-  <autoFilter ref="B3:E5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="B3:E5" totalsRowShown="0" headerRowDxfId="588" dataDxfId="586" headerRowBorderDxfId="587" tableBorderDxfId="585" totalsRowBorderDxfId="584">
+  <autoFilter ref="B3:E5"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" dataDxfId="583"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" dataDxfId="582"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" dataDxfId="581"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4" dataDxfId="580"/>
+    <tableColumn id="1" name="Column1" dataDxfId="583"/>
+    <tableColumn id="2" name="Column2" dataDxfId="582"/>
+    <tableColumn id="3" name="Column3" dataDxfId="581"/>
+    <tableColumn id="4" name="Column4" dataDxfId="580"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="579" dataDxfId="577" headerRowBorderDxfId="578" tableBorderDxfId="576" totalsRowBorderDxfId="575">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table2628" displayName="Table2628" ref="B7:H17" totalsRowShown="0" headerRowDxfId="579" dataDxfId="577" headerRowBorderDxfId="578" tableBorderDxfId="576" totalsRowBorderDxfId="575">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Resource Name" dataDxfId="574"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="In-progress" dataDxfId="573"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Done" dataDxfId="572"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Discarded / Hold" dataDxfId="571"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Hours Spent - Project" dataDxfId="570"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Hours Spent - Non Project" dataDxfId="569"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Comments" dataDxfId="568"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="574"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="573"/>
+    <tableColumn id="3" name="Done" dataDxfId="572"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="571"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="570"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="569"/>
+    <tableColumn id="7" name="Comments" dataDxfId="568"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="567" dataDxfId="565" headerRowBorderDxfId="566" tableBorderDxfId="564" totalsRowBorderDxfId="563">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table3759" displayName="Table3759" ref="B2:E4" totalsRowShown="0" headerRowDxfId="567" dataDxfId="565" headerRowBorderDxfId="566" tableBorderDxfId="564" totalsRowBorderDxfId="563">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Column1" dataDxfId="562"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Column2" dataDxfId="561"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Column3" dataDxfId="560"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column4" dataDxfId="559"/>
+    <tableColumn id="1" name="Column1" dataDxfId="562"/>
+    <tableColumn id="2" name="Column2" dataDxfId="561"/>
+    <tableColumn id="3" name="Column3" dataDxfId="560"/>
+    <tableColumn id="4" name="Column4" dataDxfId="559"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="558" dataDxfId="556" headerRowBorderDxfId="557" tableBorderDxfId="555" totalsRowBorderDxfId="554">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table262" displayName="Table262" ref="B7:H17" totalsRowShown="0" headerRowDxfId="558" dataDxfId="556" headerRowBorderDxfId="557" tableBorderDxfId="555" totalsRowBorderDxfId="554">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Resource Name" dataDxfId="553"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="In-progress" dataDxfId="552"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Done" dataDxfId="551"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Discarded / Hold" dataDxfId="550"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Hours Spent - Project" dataDxfId="549"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Hours Spent - Non Project" dataDxfId="548"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Comments" dataDxfId="547"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="553"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="552"/>
+    <tableColumn id="3" name="Done" dataDxfId="551"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="550"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="549"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="548"/>
+    <tableColumn id="7" name="Comments" dataDxfId="547"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="546" dataDxfId="544" headerRowBorderDxfId="545" tableBorderDxfId="543" totalsRowBorderDxfId="542">
-  <autoFilter ref="B2:E4" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table375" displayName="Table375" ref="B2:E4" totalsRowShown="0" headerRowDxfId="546" dataDxfId="544" headerRowBorderDxfId="545" tableBorderDxfId="543" totalsRowBorderDxfId="542">
+  <autoFilter ref="B2:E4"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Column1" dataDxfId="541"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Column2" dataDxfId="540"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Column3" dataDxfId="539"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Column4" dataDxfId="538"/>
+    <tableColumn id="1" name="Column1" dataDxfId="541"/>
+    <tableColumn id="2" name="Column2" dataDxfId="540"/>
+    <tableColumn id="3" name="Column3" dataDxfId="539"/>
+    <tableColumn id="4" name="Column4" dataDxfId="538"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="537" dataDxfId="535" headerRowBorderDxfId="536" tableBorderDxfId="534" totalsRowBorderDxfId="533">
-  <autoFilter ref="B7:H17" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2621012" displayName="Table2621012" ref="B7:H17" totalsRowShown="0" headerRowDxfId="537" dataDxfId="535" headerRowBorderDxfId="536" tableBorderDxfId="534" totalsRowBorderDxfId="533">
+  <autoFilter ref="B7:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Resource Name" dataDxfId="532"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="In-progress" dataDxfId="531"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Done" dataDxfId="530"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Discarded / Hold" dataDxfId="529"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Hours Spent - Project" dataDxfId="528"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Hours Spent - Non Project" dataDxfId="527"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Comments" dataDxfId="526"/>
+    <tableColumn id="1" name="Resource Name" dataDxfId="532"/>
+    <tableColumn id="2" name="In-progress" dataDxfId="531"/>
+    <tableColumn id="3" name="Done" dataDxfId="530"/>
+    <tableColumn id="4" name="Discarded / Hold" dataDxfId="529"/>
+    <tableColumn id="5" name="Hours Spent - Project" dataDxfId="528"/>
+    <tableColumn id="6" name="Hours Spent - Non Project" dataDxfId="527"/>
+    <tableColumn id="7" name="Comments" dataDxfId="526"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -16063,23 +16068,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -16115,23 +16103,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -16307,14 +16278,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.109375" customWidth="1"/>
     <col min="3" max="3" width="92.109375" customWidth="1"/>
@@ -16323,7 +16294,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -16340,7 +16311,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="2:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -16357,7 +16328,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="2:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -16366,7 +16337,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="2:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -16375,7 +16346,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="20.3" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="11"/>
@@ -16384,7 +16355,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="2:8" s="12" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" s="12" customFormat="1" ht="65.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
@@ -16407,7 +16378,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -16428,7 +16399,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
@@ -16449,7 +16420,7 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
@@ -16470,7 +16441,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
@@ -16491,7 +16462,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="19" t="s">
         <v>24</v>
       </c>
@@ -16512,7 +16483,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20" t="s">
         <v>27</v>
       </c>
@@ -16533,7 +16504,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -16554,7 +16525,7 @@
       </c>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
@@ -16575,7 +16546,7 @@
       </c>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -16596,7 +16567,7 @@
       </c>
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="2:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="65.3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>36</v>
       </c>
@@ -16628,14 +16599,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -16646,7 +16617,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -16663,7 +16634,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -16680,7 +16651,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -16689,7 +16660,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -16698,7 +16669,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -16707,7 +16678,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -16731,7 +16702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="219.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -16773,7 +16744,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="146.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -16794,7 +16765,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="229.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="229.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -16832,7 +16803,7 @@
       <c r="G12" s="35"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -16853,7 +16824,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -16874,7 +16845,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="196.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -16895,7 +16866,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -16914,7 +16885,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -16945,14 +16916,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -16963,7 +16934,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -16980,7 +16951,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -16997,7 +16968,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -17006,7 +16977,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -17015,7 +16986,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -17024,7 +16995,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -17048,7 +17019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="219.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -17090,7 +17061,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="146.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -17111,7 +17082,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="229.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="229.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -17149,7 +17120,7 @@
       <c r="G12" s="35"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -17170,7 +17141,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -17191,7 +17162,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="196.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -17231,7 +17202,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -17262,14 +17233,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -17280,7 +17251,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -17297,7 +17268,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -17314,7 +17285,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -17323,7 +17294,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -17332,7 +17303,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -17341,7 +17312,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -17365,7 +17336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="219.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -17386,7 +17357,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="234.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="235" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -17407,7 +17378,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="204.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -17428,7 +17399,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="229.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="229.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -17466,7 +17437,7 @@
       <c r="G12" s="35"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -17487,7 +17458,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -17508,7 +17479,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="196.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -17529,7 +17500,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -17548,7 +17519,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -17579,14 +17550,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -17597,7 +17568,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -17614,7 +17585,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -17631,7 +17602,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -17640,7 +17611,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -17649,7 +17620,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -17658,7 +17629,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -17682,7 +17653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="219.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="219.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -17703,7 +17674,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="173.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -17724,7 +17695,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="170.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="170.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -17745,7 +17716,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="179.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="179.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -17783,7 +17754,7 @@
       <c r="G12" s="35"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -17804,7 +17775,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -17825,7 +17796,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="303.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="303.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -17846,7 +17817,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -17865,7 +17836,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -17896,14 +17867,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H19"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="57.33203125" customWidth="1"/>
     <col min="3" max="3" width="72.33203125" customWidth="1"/>
@@ -17913,7 +17884,7 @@
     <col min="8" max="8" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -17930,7 +17901,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -17947,7 +17918,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="33"/>
       <c r="D6" s="7"/>
@@ -17956,7 +17927,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="34"/>
       <c r="D7" s="9"/>
@@ -17965,7 +17936,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B8" s="11"/>
       <c r="C8" s="36"/>
       <c r="D8" s="11"/>
@@ -17974,7 +17945,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="20.95" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="18" t="s">
         <v>4</v>
@@ -17998,7 +17969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="168" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="168.05" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -18019,7 +17990,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" ht="224.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="224.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
@@ -18099,7 +18070,7 @@
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="211.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="211.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
         <v>27</v>
       </c>
@@ -18120,7 +18091,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" ht="204" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="204.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -18141,7 +18112,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="2:8" ht="232.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="232.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
@@ -18162,7 +18133,7 @@
       </c>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8" ht="207.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="208" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -18181,7 +18152,7 @@
       </c>
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="2:8" ht="208.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>54</v>
       </c>
@@ -18212,14 +18183,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="57.33203125" customWidth="1"/>
     <col min="3" max="3" width="72.33203125" customWidth="1"/>
@@ -18229,7 +18200,7 @@
     <col min="8" max="8" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -18246,7 +18217,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -18263,7 +18234,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="33"/>
       <c r="D6" s="7"/>
@@ -18272,7 +18243,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="34"/>
       <c r="D7" s="9"/>
@@ -18281,7 +18252,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B8" s="11"/>
       <c r="C8" s="36"/>
       <c r="D8" s="11"/>
@@ -18290,7 +18261,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="20.95" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="18" t="s">
         <v>4</v>
@@ -18314,7 +18285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="336" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="335.95" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>13</v>
       </c>
@@ -18335,7 +18306,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" ht="348" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="348.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
@@ -18356,7 +18327,7 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="327.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="327.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
@@ -18436,7 +18407,7 @@
       </c>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" ht="395.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="395.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>30</v>
       </c>
@@ -18457,7 +18428,7 @@
       </c>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="2:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="19" t="s">
         <v>31</v>
       </c>
@@ -18478,7 +18449,7 @@
       </c>
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="2:8" ht="291.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="291.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>34</v>
       </c>
@@ -18497,7 +18468,7 @@
       </c>
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="2:8" ht="208.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>54</v>
       </c>
@@ -18528,14 +18499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H21"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="57.33203125" customWidth="1"/>
     <col min="3" max="3" width="72.33203125" customWidth="1"/>
@@ -18546,7 +18517,7 @@
     <col min="8" max="8" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -18563,7 +18534,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
@@ -18580,7 +18551,7 @@
       <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="6"/>
       <c r="C6" s="33"/>
       <c r="D6" s="7"/>
@@ -18589,7 +18560,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="34"/>
       <c r="D7" s="9"/>
@@ -18598,7 +18569,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B8" s="11"/>
       <c r="C8" s="36"/>
       <c r="D8" s="11"/>
@@ -18607,7 +18578,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="20.95" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="18" t="s">
         <v>4</v>
@@ -18652,7 +18623,7 @@
       </c>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="120.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>17</v>
       </c>
@@ -18669,7 +18640,7 @@
       <c r="G11" s="35"/>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:8" ht="373.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="373.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>263</v>
       </c>
@@ -18690,7 +18661,7 @@
       </c>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="119.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
@@ -18783,7 +18754,7 @@
       <c r="G17" s="35"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="2:8" ht="336" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" ht="335.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>276</v>
       </c>
@@ -18800,7 +18771,7 @@
       <c r="G18" s="35"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="2:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>54</v>
       </c>
@@ -18821,8 +18792,8 @@
       </c>
       <c r="H19" s="28"/>
     </row>
-    <row r="20" spans="2:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:8" ht="22.65" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:8" ht="26.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:8" ht="22.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -18833,14 +18804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q166"/>
   <sheetViews>
     <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -22248,7 +22219,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C166" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C166">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -22257,14 +22228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A71" workbookViewId="0">
       <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -22278,7 +22249,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -24871,7 +24842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -25587,7 +25558,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -25596,14 +25567,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A51" zoomScale="80" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -25617,7 +25588,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -27969,7 +27940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -28607,7 +28578,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -28616,14 +28587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="34.5546875" customWidth="1"/>
     <col min="3" max="3" width="105.33203125" style="38" customWidth="1"/>
@@ -28633,7 +28604,7 @@
     <col min="7" max="8" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -28650,7 +28621,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
@@ -28667,7 +28638,7 @@
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
       <c r="C5" s="33"/>
       <c r="D5" s="7"/>
@@ -28676,7 +28647,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="4"/>
       <c r="C6" s="34"/>
       <c r="D6" s="9"/>
@@ -28685,7 +28656,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B7" s="11"/>
       <c r="C7" s="36"/>
       <c r="D7" s="11"/>
@@ -28694,7 +28665,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="40.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="40.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="B8" s="18" t="s">
         <v>4</v>
@@ -28721,7 +28692,7 @@
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:11" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>13</v>
       </c>
@@ -28742,7 +28713,7 @@
       </c>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:11" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="146.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>17</v>
       </c>
@@ -28784,7 +28755,7 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" spans="1:11" ht="148.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="148.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
@@ -28805,7 +28776,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:11" ht="148.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="148.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>24</v>
       </c>
@@ -28826,7 +28797,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:11" ht="148.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="148.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>27</v>
       </c>
@@ -28837,7 +28808,7 @@
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:11" ht="148.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="148.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
         <v>30</v>
       </c>
@@ -28850,7 +28821,7 @@
       <c r="G15" s="35"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:11" ht="197.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="197.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>31</v>
       </c>
@@ -28871,7 +28842,7 @@
       </c>
       <c r="H16" s="26"/>
     </row>
-    <row r="17" spans="2:8" ht="183.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="183.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="19" t="s">
         <v>34</v>
       </c>
@@ -28892,7 +28863,7 @@
       </c>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="2:8" ht="145.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:8" ht="145.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
         <v>54</v>
       </c>
@@ -28913,9 +28884,9 @@
       </c>
       <c r="H18" s="28"/>
     </row>
-    <row r="19" spans="2:8" ht="188.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:8" ht="153.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:8" ht="188.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:8" ht="154" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:8" ht="120.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
@@ -28926,14 +28897,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -28947,7 +28918,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -31026,7 +30997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -31686,7 +31657,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -31695,14 +31666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A116" workbookViewId="0">
       <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -31716,7 +31687,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -33773,7 +33744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -34421,7 +34392,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -34430,14 +34401,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -34451,7 +34422,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -36718,7 +36689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -37300,7 +37271,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C151 C2:C22" xr:uid="{00000000-0002-0000-1500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C151 C2:C22">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -37309,12 +37280,12 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q152"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -37328,7 +37299,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -39859,7 +39830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="93"/>
       <c r="B122" s="55"/>
       <c r="C122" s="51"/>
@@ -40527,7 +40498,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152" xr:uid="{00000000-0002-0000-1600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -40536,14 +40507,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q152"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.6640625" customWidth="1"/>
@@ -40557,7 +40528,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -43237,7 +43208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="93"/>
       <c r="B122" s="55"/>
       <c r="C122" s="51"/>
@@ -43913,7 +43884,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152" xr:uid="{00000000-0002-0000-1700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -43922,14 +43893,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -43943,7 +43914,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -46440,7 +46411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="93"/>
       <c r="B122" s="55"/>
       <c r="C122" s="51"/>
@@ -47106,7 +47077,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152" xr:uid="{00000000-0002-0000-1800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C152">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -47115,12 +47086,12 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -47134,7 +47105,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -49498,7 +49469,7 @@
       <c r="E120" s="52"/>
       <c r="F120" s="52"/>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -50144,7 +50115,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C68:C151 C2:C66" xr:uid="{00000000-0002-0000-1900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C68:C151 C2:C66">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -50153,14 +50124,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -50174,7 +50145,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -52827,7 +52798,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -53546,7 +53517,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -53555,14 +53526,14 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A56" workbookViewId="0">
       <selection activeCell="O74" sqref="O74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -53576,7 +53547,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -56146,7 +56117,7 @@
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -56865,7 +56836,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -56874,14 +56845,14 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -56895,7 +56866,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -59444,7 +59415,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -60171,7 +60142,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -60180,12 +60151,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" customWidth="1"/>
@@ -60196,11 +60167,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -60217,7 +60188,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -60234,7 +60205,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -60243,7 +60214,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -60252,7 +60223,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -60261,7 +60232,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -60285,7 +60256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="168" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="168.05" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -60306,7 +60277,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="83.95" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -60325,7 +60296,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="105.05" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -60344,7 +60315,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="214.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="214.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -60365,7 +60336,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="189.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="190" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -60386,7 +60357,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="205.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -60407,7 +60378,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="101.45" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -60424,7 +60395,7 @@
       <c r="G14" s="35"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="126" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="121.75" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -60445,7 +60416,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="126" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="121.75" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -60466,7 +60437,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="168" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="162.35" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -60497,14 +60468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
     <sheetView topLeftCell="A107" workbookViewId="0">
       <selection activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -60518,7 +60489,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -63059,7 +63030,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -63753,7 +63724,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -63762,14 +63733,14 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J13:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="13" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -63798,14 +63769,14 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -63819,7 +63790,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -65991,7 +65962,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -66577,7 +66548,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-1F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -66587,14 +66558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83" customWidth="1"/>
@@ -66608,7 +66579,7 @@
     <col min="17" max="17" width="15.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>278</v>
       </c>
@@ -68994,7 +68965,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="93"/>
       <c r="B121" s="55"/>
       <c r="C121" s="51"/>
@@ -69264,21 +69235,21 @@
       <c r="A137" s="93" t="s">
         <v>276</v>
       </c>
-      <c r="B137" s="55" t="s">
-        <v>913</v>
+      <c r="B137" s="51" t="s">
+        <v>1080</v>
       </c>
       <c r="C137" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="D137" s="52">
-        <v>0.375</v>
+        <v>290</v>
+      </c>
+      <c r="D137" s="62">
+        <v>0.39583333333333331</v>
       </c>
       <c r="E137" s="52">
-        <v>0.39583333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F137" s="52">
         <f t="shared" si="3"/>
-        <v>2.0833333333333315E-2</v>
+        <v>4.8611111111111105E-2</v>
       </c>
       <c r="H137" s="49" t="s">
         <v>286</v>
@@ -69289,47 +69260,47 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="93"/>
-      <c r="B138" s="55" t="s">
-        <v>914</v>
-      </c>
-      <c r="C138" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="D138" s="52">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E138" s="52">
-        <v>0.60416666666666663</v>
+      <c r="B138" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C138" s="78" t="s">
+        <v>293</v>
+      </c>
+      <c r="D138" s="61">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E138" s="54">
+        <v>0.47916666666666669</v>
       </c>
       <c r="F138" s="52">
         <f t="shared" si="3"/>
-        <v>2.0833333333333259E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H138" s="53" t="s">
         <v>288</v>
       </c>
       <c r="I138" s="52">
         <f>SUMIFS(F137:F151, C137:C151,H138)</f>
-        <v>0.12499999999999994</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="93"/>
       <c r="B139" s="55" t="s">
-        <v>915</v>
+        <v>1079</v>
       </c>
       <c r="C139" s="51" t="s">
         <v>288</v>
       </c>
       <c r="D139" s="52">
+        <v>0.5</v>
+      </c>
+      <c r="E139" s="52">
         <v>0.625</v>
-      </c>
-      <c r="E139" s="52">
-        <v>0.64583333333333337</v>
       </c>
       <c r="F139" s="52">
         <f t="shared" si="3"/>
-        <v>2.083333333333337E-2</v>
+        <v>0.125</v>
       </c>
       <c r="H139" s="53" t="s">
         <v>285</v>
@@ -69341,28 +69312,20 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="93"/>
-      <c r="B140" s="55" t="s">
-        <v>916</v>
-      </c>
-      <c r="C140" s="51" t="s">
-        <v>288</v>
-      </c>
-      <c r="D140" s="52">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E140" s="52">
-        <v>0.97916666666666663</v>
-      </c>
+      <c r="B140" s="55"/>
+      <c r="C140" s="51"/>
+      <c r="D140" s="52"/>
+      <c r="E140" s="52"/>
       <c r="F140" s="52">
         <f t="shared" si="3"/>
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="H140" s="53" t="s">
         <v>290</v>
       </c>
       <c r="I140" s="52">
         <f>SUMIFS(F137:F151, C137:C151,H140)</f>
-        <v>0</v>
+        <v>4.8611111111111105E-2</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
@@ -69380,7 +69343,7 @@
       </c>
       <c r="I141" s="52">
         <f>SUMIFS(F137:F151, C137:C151,H141)</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
@@ -69434,7 +69397,7 @@
       </c>
       <c r="I144" s="49">
         <f>SUM(I138:I143)</f>
-        <v>0.12499999999999994</v>
+        <v>0.19444444444444448</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
@@ -69632,7 +69595,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151" xr:uid="{00000000-0002-0000-2000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C151">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -69641,14 +69604,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" customWidth="1"/>
@@ -69659,11 +69622,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -69680,7 +69643,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -69697,7 +69660,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -69706,7 +69669,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -69715,7 +69678,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -69724,7 +69687,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -69748,7 +69711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="20.95" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -69790,7 +69753,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="83.95" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -69811,7 +69774,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="214.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="214.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -69832,7 +69795,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="189.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="190" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -69853,7 +69816,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="205.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="205.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -69874,7 +69837,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="63" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="60.9" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -69895,7 +69858,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="101.45" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -69916,7 +69879,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="81.2" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -69937,7 +69900,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="84" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="60.9" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -69968,14 +69931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" customWidth="1"/>
@@ -69986,11 +69949,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -70007,7 +69970,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -70024,7 +69987,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -70033,7 +69996,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -70042,7 +70005,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -70051,7 +70014,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -70075,7 +70038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="103.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="103.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -70117,7 +70080,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="102.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -70138,7 +70101,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="116.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -70159,7 +70122,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -70180,7 +70143,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -70201,7 +70164,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="83.95" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -70243,7 +70206,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="110.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -70264,7 +70227,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="142.55000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -70295,14 +70258,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" customWidth="1"/>
@@ -70313,11 +70276,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -70334,7 +70297,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -70351,7 +70314,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -70360,7 +70323,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -70369,7 +70332,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -70378,7 +70341,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -70444,7 +70407,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="102.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -70465,7 +70428,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="116.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -70486,7 +70449,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -70507,7 +70470,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -70528,7 +70491,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="117.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="118" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -70549,7 +70512,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="145.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="145.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -70570,7 +70533,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="144" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" ht="144" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -70591,7 +70554,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="142.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="142.55000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -70622,14 +70585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="49.5546875" customWidth="1"/>
@@ -70640,11 +70603,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -70661,7 +70624,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -70678,7 +70641,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -70687,7 +70650,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -70696,7 +70659,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -70705,7 +70668,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -70729,7 +70692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="112.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="112.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -70771,7 +70734,7 @@
       </c>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="102.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -70792,7 +70755,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="116.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -70813,7 +70776,7 @@
       </c>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>24</v>
       </c>
@@ -70834,7 +70797,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="133.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -70855,7 +70818,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="112.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="112.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -70876,7 +70839,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="201" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="200.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -70897,7 +70860,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="146.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="146.30000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -70918,7 +70881,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="268.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="268.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -70949,14 +70912,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -70967,7 +70930,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -70984,7 +70947,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -71001,7 +70964,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -71010,7 +70973,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -71019,7 +70982,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -71028,7 +70991,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -71052,7 +71015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="243.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="244" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -71073,7 +71036,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="233.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="233.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -71092,7 +71055,7 @@
       <c r="G9" s="35"/>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="146.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -71111,7 +71074,7 @@
       <c r="G10" s="35"/>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="229.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="229.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -71153,7 +71116,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -71174,7 +71137,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -71195,7 +71158,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="196.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -71216,7 +71179,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -71237,7 +71200,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>
@@ -71268,14 +71231,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
@@ -71286,7 +71249,7 @@
     <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -71303,7 +71266,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -71320,7 +71283,7 @@
       <c r="G3" s="9"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="33"/>
       <c r="D4" s="7"/>
@@ -71329,7 +71292,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B5" s="4"/>
       <c r="C5" s="34"/>
       <c r="D5" s="9"/>
@@ -71338,7 +71301,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="20.95" x14ac:dyDescent="0.4">
       <c r="B6" s="11"/>
       <c r="C6" s="36"/>
       <c r="D6" s="11"/>
@@ -71347,7 +71310,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="42.05" x14ac:dyDescent="0.3">
       <c r="A7" s="12"/>
       <c r="B7" s="18" t="s">
         <v>4</v>
@@ -71371,7 +71334,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="243.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="244" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="19" t="s">
         <v>13</v>
       </c>
@@ -71392,7 +71355,7 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8" ht="233.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="233.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
@@ -71411,7 +71374,7 @@
       <c r="G9" s="35"/>
       <c r="H9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="146.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="19" t="s">
         <v>20</v>
       </c>
@@ -71432,7 +71395,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" spans="1:8" ht="229.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="229.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="19" t="s">
         <v>21</v>
       </c>
@@ -71474,7 +71437,7 @@
       </c>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="191.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>27</v>
       </c>
@@ -71495,7 +71458,7 @@
       </c>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>30</v>
       </c>
@@ -71516,7 +71479,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="196.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" ht="196.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19" t="s">
         <v>31</v>
       </c>
@@ -71537,7 +71500,7 @@
       </c>
       <c r="H15" s="26"/>
     </row>
-    <row r="16" spans="1:8" ht="197.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="197.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>34</v>
       </c>
@@ -71556,7 +71519,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" ht="273.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:8" ht="273.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>54</v>
       </c>

</xml_diff>